<commit_message>
Fixed errors in valume calculations for magnet insert. Added automatic update of external dewar helium volume when adding/removing He to the system
</commit_message>
<xml_diff>
--- a/doc/He_density.xlsx
+++ b/doc/He_density.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Freia\freia-drop\08 Equipment\Cryostat02_Gersemi\09 Controls and Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA3A51F-0273-42F4-8E90-8DA3FC3269FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B5BE1-3D75-400E-BF3B-C7794D3804C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7840" xr2:uid="{8EA47820-C17B-4FA3-9CFF-19528A798E56}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16330" windowHeight="7840" activeTab="1" xr2:uid="{8EA47820-C17B-4FA3-9CFF-19528A798E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Equlibrium" sheetId="1" r:id="rId1"/>
     <sheet name="Liquid" sheetId="2" r:id="rId2"/>
     <sheet name="Gas" sheetId="3" r:id="rId3"/>
+    <sheet name="CM volumes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>https://nvlpubs.nist.gov/nistpubs/Legacy/TN/nbstechnicalnote1334.pdf</t>
   </si>
@@ -259,15 +260,38 @@
   <si>
     <t>2.31e+3</t>
   </si>
+  <si>
+    <t>V [m3]</t>
+  </si>
+  <si>
+    <t>LT01/02 [cm]</t>
+  </si>
+  <si>
+    <t>LT01/02 [%]</t>
+  </si>
+  <si>
+    <t>y=2,23e-4*x</t>
+  </si>
+  <si>
+    <t>y=(x-52)*3,75+0,116</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,18 +320,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,7 +462,7 @@
                   <c:y val="0.15517315543890348"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3252,6 +3279,795 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9372703412073493E-2"/>
+          <c:y val="0.15800695249130942"/>
+          <c:w val="0.87129396325459318"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CM volumes'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V [m3]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CBCB-4105-9335-B621EA65AB4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>top level</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.3374671916010502E-2"/>
+                  <c:y val="0.13816394337990984"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$B$6:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>51.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$D$6:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CBCB-4105-9335-B621EA65AB4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="877359904"/>
+        <c:axId val="782678112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="877359904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="782678112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="782678112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="877359904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CM volumes'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V [m3]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CM volumes'!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C277-4A02-9941-1CD09FD71F8E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1025293648"/>
+        <c:axId val="780364400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1025293648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="780364400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="780364400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1025293648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -3355,11 +4171,11 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10015463692038495"/>
-                  <c:y val="-2.6472003499562555E-2"/>
+                  <c:x val="-4.9876859142607172E-2"/>
+                  <c:y val="-3.5654271539756954E-3"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3792,11 +4608,11 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.34506233595800523"/>
-                  <c:y val="-0.20810941506008157"/>
+                  <c:x val="-0.20531211723534559"/>
+                  <c:y val="-0.19967993584135316"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -4177,11 +4993,11 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.34446762904636918"/>
-                  <c:y val="0.40261373578302712"/>
+                  <c:x val="-0.14238451443569553"/>
+                  <c:y val="0.35168780985710119"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -7242,6 +8058,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9627,6 +10523,1038 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14759,6 +16687,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>26987</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>74612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>331787</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4A569E-123D-4F69-8839-6331BD7FC195}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1046162</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>284162</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>131762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE67892-C2A9-4BE6-A363-F879ABDEE28C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15058,14 +17063,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4E8205-3E82-42A2-8AA2-F2CDB40EF2EF}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Y48" sqref="Y48"/>
-    </sheetView>
+    <sheetView topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15521,8 +17524,11 @@
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{9C9B0232-EC0E-40B6-9BBD-D56EF02A82E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15530,8 +17536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64BB1C-42FB-4891-951D-FE7A4A7C035C}">
   <dimension ref="B2:Y43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16049,7 +18055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6154F659-BFE1-45A1-A0D5-E5BBAF1CBB15}">
   <dimension ref="A2:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -16569,4 +18575,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A49F61-C3CD-4E2F-91F2-B82B92067C5F}">
+  <dimension ref="B3:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>B4/68</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>0.00223*B4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>24.8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C8" si="0">B5/68</f>
+        <v>0.36470588235294121</v>
+      </c>
+      <c r="D5">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E6" si="1">0.00223*B5</f>
+        <v>5.5304000000000006E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>51.9</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.76323529411764701</v>
+      </c>
+      <c r="D6">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.11573700000000001</v>
+      </c>
+      <c r="F6">
+        <f>(B6-52)*0.0003+0.116</f>
+        <v>0.11597</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.98529411764705888</v>
+      </c>
+      <c r="D7">
+        <v>0.12</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F8" si="2">(B7-52)*0.0003+0.116</f>
+        <v>0.12050000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.122</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.1208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug in calculating LHe mass in D5200. Changed the calculation fo GHe mass in D5200.
</commit_message>
<xml_diff>
--- a/doc/He_density.xlsx
+++ b/doc/He_density.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Freia\freia-drop\08 Equipment\Cryostat02_Gersemi\09 Controls and Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B5BE1-3D75-400E-BF3B-C7794D3804C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EDE732-B4B0-455D-83F8-B6C6155B56E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16330" windowHeight="7840" activeTab="1" xr2:uid="{8EA47820-C17B-4FA3-9CFF-19528A798E56}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26940" windowHeight="10310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equlibrium" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Konrad Gajewski</author>
+  </authors>
+  <commentList>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Konrad Gajewski:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LHe density at atmospheric pressure</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>https://nvlpubs.nist.gov/nistpubs/Legacy/TN/nbstechnicalnote1334.pdf</t>
   </si>
@@ -275,12 +309,15 @@
   <si>
     <t>y=(x-52)*3,75+0,116</t>
   </si>
+  <si>
+    <t>Density at 300 K and 1 bar: 0.1598 kg/m3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +333,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,14 +380,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -814,6 +871,780 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Density vs Pressure</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1.8K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24387817147856519"/>
+                  <c:y val="-5.590751445086705E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Liquid!$O$19:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Liquid!$P$19:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>147.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>147.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8144-439D-96A2-592C84A52EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24387817147856519"/>
+                  <c:y val="8.8323699421965322E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Liquid!$O$19:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Liquid!$Q$19:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>147.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>148.19999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8144-439D-96A2-592C84A52EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24665594925634296"/>
+                  <c:y val="2.4099039643165992E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Liquid!$O$19:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Liquid!$U$19:$U$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>143.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144.30000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8144-439D-96A2-592C84A52EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>4.2K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.22443372703412073"/>
+                  <c:y val="4.8424559646807072E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Liquid!$O$19:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Liquid!$Y$19:$Y$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>125.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8144-439D-96A2-592C84A52EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1030089600"/>
+        <c:axId val="869756400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1030089600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="869756400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="869756400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1030089600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1328,7 +2159,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1970,7 +2801,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2897,7 +3728,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3279,7 +4110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3708,7 +4539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6052,6 +6883,404 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Liquid Density [kg/m3] vs Pressure [bar] (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>for D5200)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Liquid</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.20531211723534559"/>
+                  <c:y val="-0.19967993584135316"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Equlibrium!$E$15:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.82599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Equlibrium!$B$15:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>128.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8396-4FA2-ABC7-1FACCCF6D3F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="779767824"/>
+        <c:axId val="781393504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="779767824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="781393504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="781393504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="779767824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent4">
+        <a:lumMod val="40000"/>
+        <a:lumOff val="60000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -6559,7 +7788,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6973,7 +8202,7 @@
         <c:axId val="1028873696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="120"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7029,780 +8258,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1023757904"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="sv-SE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="sv-SE"/>
-              <a:t>Density vs Pressure</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sv-SE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>1.8K</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.24387817147856519"/>
-                  <c:y val="-5.590751445086705E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="sv-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Liquid!$O$19:$O$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Liquid!$P$19:$P$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>147.19999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>147.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>147.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8144-439D-96A2-592C84A52EC8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>2K</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.24387817147856519"/>
-                  <c:y val="8.8323699421965322E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="sv-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Liquid!$O$19:$O$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Liquid!$Q$19:$Q$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>147.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>147.9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>148.19999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8144-439D-96A2-592C84A52EC8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>3K</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.24665594925634296"/>
-                  <c:y val="2.4099039643165992E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="sv-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Liquid!$O$19:$O$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Liquid!$U$19:$U$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>143.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>143.80000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>144.30000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8144-439D-96A2-592C84A52EC8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>4.2K</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.22443372703412073"/>
-                  <c:y val="4.8424559646807072E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="sv-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Liquid!$O$19:$O$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Liquid!$Y$19:$Y$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>125.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>126.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>127.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8144-439D-96A2-592C84A52EC8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1030089600"/>
-        <c:axId val="869756400"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1030089600"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="sv-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="869756400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="869756400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="sv-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1030089600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8099,6 +8554,46 @@
 </file>
 
 <file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12070,6 +12565,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -16274,16 +17285,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16310,16 +17321,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>358775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16348,16 +17359,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16387,15 +17398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16417,6 +17428,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24712DEF-711F-4093-9406-9688D57F3B3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17060,23 +18109,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4E8205-3E82-42A2-8AA2-F2CDB40EF2EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -17254,7 +18305,7 @@
       <c r="A16">
         <v>4.25</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>124.4</v>
       </c>
       <c r="C16">
@@ -17525,29 +18576,30 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{9C9B0232-EC0E-40B6-9BBD-D56EF02A82E3}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64BB1C-42FB-4891-951D-FE7A4A7C035C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -18052,21 +19104,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6154F659-BFE1-45A1-A0D5-E5BBAF1CBB15}">
-  <dimension ref="A2:J21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2">
         <v>58</v>
       </c>
@@ -18438,7 +19490,7 @@
         <v>6.4180000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>600</v>
       </c>
@@ -18464,7 +19516,7 @@
         <v>9.6259999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>800</v>
       </c>
@@ -18490,7 +19542,7 @@
         <v>0.1283</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1013</v>
       </c>
@@ -18516,7 +19568,7 @@
         <v>0.16250000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1200</v>
       </c>
@@ -18541,8 +19593,11 @@
       <c r="H20" s="2">
         <v>0.1925</v>
       </c>
+      <c r="K20" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1400</v>
       </c>
@@ -18578,7 +19633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A49F61-C3CD-4E2F-91F2-B82B92067C5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18587,8 +19642,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="2" max="3" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>